<commit_message>
Implement performance measurement code
</commit_message>
<xml_diff>
--- a/measurements/TTT_Graphs.xlsx
+++ b/measurements/TTT_Graphs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\saxion\dotnet\ttt_embedding_languages\measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03972B4-6630-43FE-AAA2-BE528B386174}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE30A22-9978-46E0-9FA5-FC1D2BE3B772}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{410AF11E-6A3D-47BB-A088-0867356F1991}"/>
   </bookViews>
@@ -942,13 +942,13 @@
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400"/>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>(microseconds/write)</a:t>
+              <a:t>(microseconds/write int)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1620,23 +1620,20 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>(microseconds/read)</a:t>
+              <a:t>(microseconds/read int)</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB" sz="1400">
               <a:effectLst/>
@@ -5001,8 +4998,8 @@
       <xdr:rowOff>179294</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>73959</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>10165</xdr:rowOff>
     </xdr:to>
@@ -5109,8 +5106,8 @@
       <xdr:rowOff>141195</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>215153</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>358588</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>162566</xdr:rowOff>
     </xdr:to>
@@ -5440,7 +5437,7 @@
   <dimension ref="B3:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5927,7 +5924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC9E7BB-7480-4FD3-897A-98517A81AF40}">
   <dimension ref="B3:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add python graphs for basic measurements
</commit_message>
<xml_diff>
--- a/measurements/TTT_Graphs.xlsx
+++ b/measurements/TTT_Graphs.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\saxion\dotnet\ttt_embedding_languages\measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE30A22-9978-46E0-9FA5-FC1D2BE3B772}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1373DD4B-47A0-415B-83C8-087F48CDA5B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{410AF11E-6A3D-47BB-A088-0867356F1991}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{410AF11E-6A3D-47BB-A088-0867356F1991}"/>
   </bookViews>
   <sheets>
     <sheet name="Lua" sheetId="1" r:id="rId1"/>
@@ -2816,6 +2816,2419 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Python - Read Memory Usage</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(bytes/read int)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Normal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0\ \B" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>Get/Set</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Exec/Eval</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Python!$G$7,Python!$G$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>72.0023193359375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.0159912109375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-C3AF-4E7A-8100-A26943C3060E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Garbage Collected</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0\ \B" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>(Python!$G$8,Python!$G$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>72.0030517578125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.0030517578125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-C3AF-4E7A-8100-A26943C3060E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="-10"/>
+        <c:axId val="1850924688"/>
+        <c:axId val="1850926352"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1850924688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1850926352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1850926352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="120"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Bytes/read</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1850924688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="10"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Python - Write Memory Usage</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(bytes/write int)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Normal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0\ \B" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>Get/Set</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Exec/Eval</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Python!$G$5,Python!$G$9)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>48.076171875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>102.7786865234375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-C3AF-4E7A-8100-A26943C3060E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Garbage Collected</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0\ \B" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>(Python!$G$6,Python!$G$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>48.0052490234375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>102.778076171875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-C3AF-4E7A-8100-A26943C3060E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="-10"/>
+        <c:axId val="1850924688"/>
+        <c:axId val="1850926352"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1850924688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1850926352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1850926352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="120"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Bytes/write</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1850924688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="10"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Python - Write Performance</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(microseconds/write int)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Min</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00\ \µ\s" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Lua!$C$19,Lua!$C$21)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Get/Set</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Exec/Eval</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Python!$L$19,Python!$L$21)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.12476501464843751</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6415451049804686</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D5BC-4D80-9C0F-C8F3BAA1E58F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Max</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00\ \µ\s" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>(Python!$M$19,Python!$M$21)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.25105743408203124</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0528930664062504</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D5BC-4D80-9C0F-C8F3BAA1E58F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Average</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00\ \µ\s" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>(Python!$N$19,Python!$N$21)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.13490753173828127</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.8746902465820305</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D5BC-4D80-9C0F-C8F3BAA1E58F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="-10"/>
+        <c:axId val="812473455"/>
+        <c:axId val="812477199"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="812473455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="812477199"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="812477199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>µs/write</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="812473455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:minorUnit val="0.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Python - Write Performance</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(microseconds/read int)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Min</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00\ \µ\s" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Lua!$C$19,Lua!$C$21)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Get/Set</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Exec/Eval</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Python!$L$20,Python!$L$22)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.236297607421875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.7024124145507811</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D5BC-4D80-9C0F-C8F3BAA1E58F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Max</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00\ \µ\s" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>(Python!$M$20,Python!$M$22)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.44258422851562496</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8944427490234377</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D5BC-4D80-9C0F-C8F3BAA1E58F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Average</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00\ \µ\s" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>(Python!$N$20,Python!$N$22)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.27984008789062503</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.7835357666015632</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D5BC-4D80-9C0F-C8F3BAA1E58F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="-10"/>
+        <c:axId val="812473455"/>
+        <c:axId val="812477199"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="812473455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="812477199"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="812477199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="9"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>µs/read</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="812473455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
+        <c:minorUnit val="0.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2976,6 +5389,166 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4486,6 +7059,2018 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5121,6 +9706,159 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>521071</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>44825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>50424</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>121025</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DB92696-C5D5-47A2-892A-E430DE1D4AA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12325</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>6724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>292472</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>82924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8D864CF-E11A-4BFC-8680-59D93D56C868}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>17928</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>17930</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>268940</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>94130</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7469E1F2-ED3B-4CDF-9C1B-E7AEB1A3E714}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>573738</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>58271</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>33616</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A45C4D3C-29F8-4FE7-9417-3751AB2BF8AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -5434,10 +10172,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9031561D-9105-4EF0-AA0D-80076824960E}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X41" sqref="X41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5922,10 +10661,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC9E7BB-7480-4FD3-897A-98517A81AF40}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:N22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q46" sqref="Q46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6404,5 +11144,6 @@
     <mergeCell ref="E17:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add comparison charts for complex data types
</commit_message>
<xml_diff>
--- a/measurements/TTT_Graphs.xlsx
+++ b/measurements/TTT_Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\saxion\dotnet\ttt_embedding_languages\measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6F5165-0872-4D73-8A87-1E6F1DB8C3FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43CBDE1-5A3F-4BF9-972C-97943383AE58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{410AF11E-6A3D-47BB-A088-0867356F1991}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="36">
   <si>
     <t>TYPE</t>
   </si>
@@ -101,22 +101,59 @@
     <t>PER-ACTION (ns)</t>
   </si>
   <si>
-    <t>TIME LUA</t>
+    <t>TIME LUA - BASIC</t>
   </si>
   <si>
-    <t>TIME PYTHON</t>
+    <t>TIME PYTHON - BASIC</t>
   </si>
   <si>
-    <t>Memory LUA</t>
+    <t>Memory LUA - BASIC</t>
   </si>
   <si>
-    <t>Memory PYTHON</t>
+    <t>Memory PYTHON - BASIC</t>
+  </si>
+  <si>
+    <t>lang</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>1MB object</t>
+  </si>
+  <si>
+    <t>Vector3 struct</t>
+  </si>
+  <si>
+    <t>Transform struct (3 x Vector3)</t>
+  </si>
+  <si>
+    <t>Write Complex</t>
+  </si>
+  <si>
+    <t>lua ms</t>
+  </si>
+  <si>
+    <t>python ms</t>
+  </si>
+  <si>
+    <t>lua bytes</t>
+  </si>
+  <si>
+    <t>python bytes</t>
+  </si>
+  <si>
+    <t>writes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="172" formatCode="0.000000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -296,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -336,6 +373,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -1411,6 +1456,1275 @@
         <c:crossBetween val="between"/>
         <c:majorUnit val="25"/>
         <c:minorUnit val="12.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Memory Usage</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> of writing complex types</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-GB" baseline="0"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>(bytes/write)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Lua</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:numFmt formatCode="###0\ \B" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:alpha val="32000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-3B23-4C13-ADDC-AC3CBE2F3ED8}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="###0\ \B" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>int</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Vector3</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Transform (3 x Vector3)</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1MB object</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$J$36:$M$36</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>192.3671875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>508.1640625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>535.380859375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7034.701171875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3B23-4C13-ADDC-AC3CBE2F3ED8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Python</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="###0\ \B" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>int</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Vector3</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Transform (3 x Vector3)</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1MB object</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$J$37:$M$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>48.005813598632798</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>616.236671447753</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>576.04959106445301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512.05469512939396</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3B23-4C13-ADDC-AC3CBE2F3ED8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-25"/>
+        <c:axId val="1544197872"/>
+        <c:axId val="1544210352"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1544197872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1544210352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1544210352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="700"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>bytes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0\ \B" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1544197872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:minorUnit val="50"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Performance </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>of writing complex types</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-GB" baseline="0"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>(microseconds/write)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Lua</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:numFmt formatCode="#,##0.00\ \µ\s" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:alpha val="23000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-3B23-4C13-ADDC-AC3CBE2F3ED8}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.00\ \µ\s" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>int</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Vector3</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Transform (3 x Vector3)</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1MB object</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$J$41:$M$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>20.872656249999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.728723144531251</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.720373535156249</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>700.81475830078125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3B23-4C13-ADDC-AC3CBE2F3ED8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Python</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00\ \µ\s" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>int</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Vector3</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Transform (3 x Vector3)</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1MB object</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$J$42:$M$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.20871582031249999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90682373046874998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.897216796875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85960693359374996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3B23-4C13-ADDC-AC3CBE2F3ED8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="91"/>
+        <c:overlap val="-39"/>
+        <c:axId val="1544197872"/>
+        <c:axId val="1544210352"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1544197872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1544210352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1544210352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="25"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>µs</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0\ \µ\s" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1544197872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:minorUnit val="2.5"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -6463,6 +7777,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -7287,6 +8681,1012 @@
 </file>
 
 <file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -12193,6 +14593,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>341549</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88807</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>478259</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95734</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EE91728-9CD9-4ABC-ABC1-84F444436338}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>671562</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>93850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>172182</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>100777</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FB778B6-7D3D-4CA2-AB61-DF54DA050C40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -12985,8 +15457,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:N22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G8"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13471,10 +15943,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC80D5E-FFBA-4A31-8113-D120E3FA18FB}">
-  <dimension ref="B34:G59"/>
+  <dimension ref="B34:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="E3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13484,17 +15956,24 @@
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="13" width="16.7109375" customWidth="1"/>
+    <col min="8" max="11" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="28.140625" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="34" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
+      <c r="I34" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
     </row>
-    <row r="35" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
         <v>6</v>
       </c>
@@ -13513,8 +15992,23 @@
       <c r="G35" s="23" t="s">
         <v>20</v>
       </c>
+      <c r="I35" t="s">
+        <v>25</v>
+      </c>
+      <c r="J35" t="s">
+        <v>26</v>
+      </c>
+      <c r="K35" t="s">
+        <v>28</v>
+      </c>
+      <c r="L35" t="s">
+        <v>29</v>
+      </c>
+      <c r="M35" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
@@ -13527,8 +16021,23 @@
       <c r="G36" s="17" t="s">
         <v>11</v>
       </c>
+      <c r="I36" t="s">
+        <v>33</v>
+      </c>
+      <c r="J36" s="26">
+        <v>192.3671875</v>
+      </c>
+      <c r="K36" s="26">
+        <v>508.1640625</v>
+      </c>
+      <c r="L36" s="26">
+        <v>535.380859375</v>
+      </c>
+      <c r="M36" s="26">
+        <v>7034.701171875</v>
+      </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="11">
         <v>65536</v>
       </c>
@@ -13549,8 +16058,23 @@
         <f>F37*1000*1000</f>
         <v>209.15679931640625</v>
       </c>
+      <c r="I37" t="s">
+        <v>34</v>
+      </c>
+      <c r="J37" s="26">
+        <v>48.005813598632798</v>
+      </c>
+      <c r="K37" s="26">
+        <v>616.236671447753</v>
+      </c>
+      <c r="L37" s="26">
+        <v>576.04959106445301</v>
+      </c>
+      <c r="M37" s="26">
+        <v>512.05469512939396</v>
+      </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="13">
         <v>65536</v>
       </c>
@@ -13571,15 +16095,71 @@
         <f>F38*1000*1000</f>
         <v>189.5355224609375</v>
       </c>
+      <c r="I38" t="s">
+        <v>31</v>
+      </c>
+      <c r="J38" s="25">
+        <v>170.9888</v>
+      </c>
+      <c r="K38" s="25">
+        <v>178.0017</v>
+      </c>
+      <c r="L38" s="25">
+        <v>177.9333</v>
+      </c>
+      <c r="M38" s="25">
+        <v>5741.0744999999997</v>
+      </c>
     </row>
-    <row r="41" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>32</v>
+      </c>
+      <c r="J39" s="25">
+        <v>1.7098</v>
+      </c>
+      <c r="K39" s="25">
+        <v>7.4287000000000001</v>
+      </c>
+      <c r="L39" s="25">
+        <v>7.35</v>
+      </c>
+      <c r="M39" s="25">
+        <v>7.0419</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I40" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J40" s="28">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
+      <c r="J41">
+        <f>J38/$J$40*1000</f>
+        <v>20.872656249999999</v>
+      </c>
+      <c r="K41">
+        <f t="shared" ref="K41:M41" si="0">K38/$J$40*1000</f>
+        <v>21.728723144531251</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="0"/>
+        <v>21.720373535156249</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="0"/>
+        <v>700.81475830078125</v>
+      </c>
     </row>
-    <row r="42" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B42" s="18" t="s">
         <v>6</v>
       </c>
@@ -13598,8 +16178,24 @@
       <c r="G42" s="23" t="s">
         <v>15</v>
       </c>
+      <c r="J42">
+        <f>J39/$J$40*1000</f>
+        <v>0.20871582031249999</v>
+      </c>
+      <c r="K42">
+        <f t="shared" ref="K42:M42" si="1">K39/$J$40*1000</f>
+        <v>0.90682373046874998</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="1"/>
+        <v>0.897216796875</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="1"/>
+        <v>0.85960693359374996</v>
+      </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
@@ -13613,7 +16209,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="11">
         <v>65536</v>
       </c>
@@ -13635,7 +16231,7 @@
         <v>134.90753173828128</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" s="13">
         <v>65536</v>
       </c>
@@ -13722,7 +16318,7 @@
         <v>11534400</v>
       </c>
       <c r="G53" s="7">
-        <f t="shared" ref="G53" si="0">F53/B53</f>
+        <f t="shared" ref="G53" si="2">F53/B53</f>
         <v>176.0009765625</v>
       </c>
     </row>
@@ -13791,14 +16387,15 @@
         <v>4718744</v>
       </c>
       <c r="G59" s="7">
-        <f t="shared" ref="G59" si="1">F59/B59</f>
+        <f t="shared" ref="G59" si="3">F59/B59</f>
         <v>72.0023193359375</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="B50:D50"/>
     <mergeCell ref="B56:D56"/>
+    <mergeCell ref="I34:K34"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="C42:C43"/>

</xml_diff>

<commit_message>
Add measurements & graphs for function calls
</commit_message>
<xml_diff>
--- a/measurements/TTT_Graphs.xlsx
+++ b/measurements/TTT_Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\saxion\dotnet\ttt_embedding_languages\measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43CBDE1-5A3F-4BF9-972C-97943383AE58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD6274D-2E96-4FE5-93C5-927E6D26C9D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{410AF11E-6A3D-47BB-A088-0867356F1991}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="40">
   <si>
     <t>TYPE</t>
   </si>
@@ -98,9 +98,6 @@
     <t>PER-ACTION (bytes)</t>
   </si>
   <si>
-    <t>PER-ACTION (ns)</t>
-  </si>
-  <si>
     <t>TIME LUA - BASIC</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
   </si>
   <si>
     <t>int</t>
-  </si>
-  <si>
-    <t>1MB object</t>
   </si>
   <si>
     <t>Vector3 struct</t>
@@ -145,14 +139,33 @@
   <si>
     <t>writes</t>
   </si>
+  <si>
+    <t>4MB object</t>
+  </si>
+  <si>
+    <t>lua microsecs</t>
+  </si>
+  <si>
+    <t>python microsecs</t>
+  </si>
+  <si>
+    <t>FUNCTION CALLS</t>
+  </si>
+  <si>
+    <t>corrected 
+(allocation of 2 ints, 1 long, 1 DateTime)</t>
+  </si>
+  <si>
+    <t>in MB / sec</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="172" formatCode="0.000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -333,7 +346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -356,6 +369,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -371,15 +394,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1759,7 +1778,7 @@
                 <c:v>Transform (3 x Vector3)</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>1MB object</c:v>
+                <c:v>4MB object</c:v>
               </c:pt>
             </c:strLit>
           </c:cat>
@@ -1878,7 +1897,7 @@
                 <c:v>Transform (3 x Vector3)</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>1MB object</c:v>
+                <c:v>4MB object</c:v>
               </c:pt>
             </c:strLit>
           </c:cat>
@@ -2392,7 +2411,7 @@
                 <c:v>Transform (3 x Vector3)</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>1MB object</c:v>
+                <c:v>4MB object</c:v>
               </c:pt>
             </c:strLit>
           </c:cat>
@@ -2511,7 +2530,7 @@
                 <c:v>Transform (3 x Vector3)</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>1MB object</c:v>
+                <c:v>4MB object</c:v>
               </c:pt>
             </c:strLit>
           </c:cat>
@@ -2653,7 +2672,7 @@
                   <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>µs</a:t>
+                  <a:t>microseconds</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -2725,6 +2744,1567 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="2.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Integer Write/Read Memory Usage</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(bytes/action)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Lua</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.0\ \B" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>Write</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Read</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Comparison!$G$52,Comparison!$G$53)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>176.019775390625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>176.0009765625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5A90-454E-A092-9973BD95B5A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Python</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.0\ \B" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>Write</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Read</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Comparison!$G$58,Comparison!$G$59)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>48.076171875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.0023193359375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5A90-454E-A092-9973BD95B5A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="-10"/>
+        <c:axId val="1850924688"/>
+        <c:axId val="1850926352"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1850924688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1850926352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1850926352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="200"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>bytes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0\ \B" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1850924688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="25"/>
+        <c:minorUnit val="12.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>1 Million Function Calls</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-GB"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Memory Usage</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> (MB)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Lua</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00\ \M\B" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$L$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>208.00001262500001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-65B6-46C5-8829-EEEFCA7A89C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Python</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00\ \M\B" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$L$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>184.007694375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-65B6-46C5-8829-EEEFCA7A89C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="414213504"/>
+        <c:axId val="414212672"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="414213504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="414212672"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="414212672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>megabytes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0\ \M\B" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="414213504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:minorUnit val="25"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>1 Million Function Calls</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-GB"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Performance </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>(seconds)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Lua</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="###0.0000\ \s" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$L$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.21245449999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-65B6-46C5-8829-EEEFCA7A89C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Python</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="###0.0000\ \s" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$L$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.0312354000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-65B6-46C5-8829-EEEFCA7A89C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="414213504"/>
+        <c:axId val="414212672"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="414213504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="414212672"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="414212672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.0\ \s" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="414213504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -7182,7 +8762,7 @@
               <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>(nanoseconds/action)</a:t>
+              <a:t>(microseconds/action)</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB" sz="1400">
               <a:effectLst/>
@@ -7243,7 +8823,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="#,##0.00\ \n\s" sourceLinked="0"/>
+            <c:numFmt formatCode="#,##0.00\ \µ\s" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -7319,10 +8899,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>209.15679931640625</c:v>
+                  <c:v>0.20915679931640624</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>189.5355224609375</c:v>
+                  <c:v>0.18953552246093749</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7350,7 +8930,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="#,##0.00\ \n\s" sourceLinked="0"/>
+            <c:numFmt formatCode="#,##0.0\ \µ\s" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -7426,10 +9006,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>134.90753173828128</c:v>
+                  <c:v>0.13490753173828127</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>279.84008789062506</c:v>
+                  <c:v>0.27984008789062503</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7509,8 +9089,7 @@
         <c:axId val="1850926352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="300"/>
-          <c:min val="0"/>
+          <c:max val="0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -7549,7 +9128,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>nanoseconds</a:t>
+                  <a:t>microseconds</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -7583,7 +9162,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="#,##0\ \n\s" sourceLinked="0"/>
+        <c:numFmt formatCode="#,##0.0\ \µ\s" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
@@ -7619,7 +9198,7 @@
         <c:crossAx val="1850924688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:minorUnit val="25"/>
+        <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -7818,6 +9397,126 @@
 </file>
 
 <file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10189,6 +11888,1515 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -14520,15 +17728,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>30307</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>143945</xdr:rowOff>
+      <xdr:colOff>20782</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>861784</xdr:colOff>
+      <xdr:colOff>852259</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>43907</xdr:rowOff>
+      <xdr:rowOff>15332</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14566,7 +17774,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>879713</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>109716</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14596,15 +17804,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>341549</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88807</xdr:rowOff>
+      <xdr:colOff>149929</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>7004</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>478259</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>95734</xdr:rowOff>
+      <xdr:colOff>615203</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>13931</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14631,16 +17839,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>671562</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>93850</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>162815</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>15409</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>172182</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>100777</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>627140</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>22336</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14660,6 +17868,116 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>600686</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>133554</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>146288</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>33516</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B8E5C72-158A-4944-B322-34DA1C29819D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>870858</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5599568C-D78D-451A-BEE6-592209CC5C15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>861333</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>8844</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{271FBE10-35B8-4B73-8F5C-FB46C8F317DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -14984,11 +18302,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -15179,46 +18497,46 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
     </row>
     <row r="17" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18" t="s">
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="19" t="s">
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="20"/>
-      <c r="N17" s="21"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="27"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
       <c r="F18" s="1" t="s">
         <v>9</v>
       </c>
@@ -15473,11 +18791,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -15668,46 +18986,46 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
     </row>
     <row r="17" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18" t="s">
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="19" t="s">
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="20"/>
-      <c r="N17" s="21"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="27"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
       <c r="F18" s="1" t="s">
         <v>9</v>
       </c>
@@ -15945,8 +19263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC80D5E-FFBA-4A31-8113-D120E3FA18FB}">
   <dimension ref="B34:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15956,62 +19274,63 @@
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="11" width="16.7109375" customWidth="1"/>
+    <col min="8" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="25" customWidth="1"/>
     <col min="12" max="12" width="28.140625" customWidth="1"/>
     <col min="13" max="13" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="34" spans="2:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="I34" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="J34" s="22"/>
-      <c r="K34" s="22"/>
+      <c r="B34" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="I34" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
     </row>
     <row r="35" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E35" s="24" t="s">
+      <c r="E35" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="24" t="s">
+      <c r="F35" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G35" s="23" t="s">
-        <v>20</v>
+      <c r="G35" s="18" t="s">
+        <v>15</v>
       </c>
       <c r="I35" t="s">
+        <v>24</v>
+      </c>
+      <c r="J35" t="s">
         <v>25</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>26</v>
       </c>
-      <c r="K35" t="s">
-        <v>28</v>
-      </c>
       <c r="L35" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M35" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
       <c r="E36" s="17" t="s">
         <v>11</v>
       </c>
@@ -16022,18 +19341,18 @@
         <v>11</v>
       </c>
       <c r="I36" t="s">
-        <v>33</v>
-      </c>
-      <c r="J36" s="26">
+        <v>31</v>
+      </c>
+      <c r="J36" s="21">
         <v>192.3671875</v>
       </c>
-      <c r="K36" s="26">
+      <c r="K36" s="21">
         <v>508.1640625</v>
       </c>
-      <c r="L36" s="26">
+      <c r="L36" s="21">
         <v>535.380859375</v>
       </c>
-      <c r="M36" s="26">
+      <c r="M36" s="21">
         <v>7034.701171875</v>
       </c>
     </row>
@@ -16055,22 +19374,22 @@
         <v>2.0915679931640625E-4</v>
       </c>
       <c r="G37" s="4">
-        <f>F37*1000*1000</f>
-        <v>209.15679931640625</v>
+        <f>F37*1000</f>
+        <v>0.20915679931640624</v>
       </c>
       <c r="I37" t="s">
-        <v>34</v>
-      </c>
-      <c r="J37" s="26">
+        <v>32</v>
+      </c>
+      <c r="J37" s="21">
         <v>48.005813598632798</v>
       </c>
-      <c r="K37" s="26">
+      <c r="K37" s="21">
         <v>616.236671447753</v>
       </c>
-      <c r="L37" s="26">
+      <c r="L37" s="21">
         <v>576.04959106445301</v>
       </c>
-      <c r="M37" s="26">
+      <c r="M37" s="21">
         <v>512.05469512939396</v>
       </c>
     </row>
@@ -16091,57 +19410,60 @@
         <f>E38/$B38</f>
         <v>1.895355224609375E-4</v>
       </c>
-      <c r="G38" s="10">
-        <f>F38*1000*1000</f>
-        <v>189.5355224609375</v>
+      <c r="G38" s="4">
+        <f>F38*1000</f>
+        <v>0.18953552246093749</v>
       </c>
       <c r="I38" t="s">
-        <v>31</v>
-      </c>
-      <c r="J38" s="25">
+        <v>29</v>
+      </c>
+      <c r="J38" s="20">
         <v>170.9888</v>
       </c>
-      <c r="K38" s="25">
+      <c r="K38" s="20">
         <v>178.0017</v>
       </c>
-      <c r="L38" s="25">
+      <c r="L38" s="20">
         <v>177.9333</v>
       </c>
-      <c r="M38" s="25">
+      <c r="M38" s="20">
         <v>5741.0744999999997</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I39" t="s">
-        <v>32</v>
-      </c>
-      <c r="J39" s="25">
+        <v>30</v>
+      </c>
+      <c r="J39" s="20">
         <v>1.7098</v>
       </c>
-      <c r="K39" s="25">
+      <c r="K39" s="20">
         <v>7.4287000000000001</v>
       </c>
-      <c r="L39" s="25">
+      <c r="L39" s="20">
         <v>7.35</v>
       </c>
-      <c r="M39" s="25">
+      <c r="M39" s="20">
         <v>7.0419</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I40" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="J40" s="28">
+      <c r="I40" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="J40" s="23">
         <v>8192</v>
       </c>
     </row>
     <row r="41" spans="2:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
+      <c r="B41" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="I41" t="s">
+        <v>35</v>
+      </c>
       <c r="J41">
         <f>J38/$J$40*1000</f>
         <v>20.872656249999999</v>
@@ -16160,23 +19482,26 @@
       </c>
     </row>
     <row r="42" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="18" t="s">
+      <c r="B42" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="18" t="s">
+      <c r="D42" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E42" s="24" t="s">
+      <c r="E42" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="24" t="s">
+      <c r="F42" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G42" s="23" t="s">
+      <c r="G42" s="18" t="s">
         <v>15</v>
+      </c>
+      <c r="I42" t="s">
+        <v>36</v>
       </c>
       <c r="J42">
         <f>J39/$J$40*1000</f>
@@ -16196,9 +19521,9 @@
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
       <c r="E43" s="17" t="s">
         <v>11</v>
       </c>
@@ -16227,8 +19552,8 @@
         <v>1.3490753173828126E-4</v>
       </c>
       <c r="G44" s="4">
-        <f>F44*1000*1000</f>
-        <v>134.90753173828128</v>
+        <f>F44*1000</f>
+        <v>0.13490753173828127</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
@@ -16248,19 +19573,72 @@
         <f>E45/$B45</f>
         <v>2.7984008789062501E-4</v>
       </c>
-      <c r="G45" s="10">
-        <f>F45*1000*1000</f>
-        <v>279.84008789062506</v>
+      <c r="G45" s="4">
+        <f>F45*1000</f>
+        <v>0.27984008789062503</v>
       </c>
     </row>
-    <row r="50" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
+    <row r="47" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
+        <v>37</v>
+      </c>
+      <c r="K47" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="L47" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="51" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
+        <v>31</v>
+      </c>
+      <c r="J48">
+        <v>232000012.625</v>
+      </c>
+      <c r="K48">
+        <f>J48-24000000</f>
+        <v>208000012.625</v>
+      </c>
+      <c r="L48">
+        <f>K48/1000000</f>
+        <v>208.00001262500001</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I49" t="s">
+        <v>32</v>
+      </c>
+      <c r="J49">
+        <v>208007694.375</v>
+      </c>
+      <c r="K49">
+        <f>J49-24000000</f>
+        <v>184007694.375</v>
+      </c>
+      <c r="L49">
+        <f>K49/1000000</f>
+        <v>184.007694375</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="I50" t="s">
+        <v>29</v>
+      </c>
+      <c r="J50">
+        <v>212.4545</v>
+      </c>
+      <c r="L50">
+        <f>J50/1000</f>
+        <v>0.21245449999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B51" s="17" t="s">
         <v>6</v>
       </c>
@@ -16279,8 +19657,18 @@
       <c r="G51" s="17" t="s">
         <v>19</v>
       </c>
+      <c r="I51" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J51">
+        <v>1031.2354</v>
+      </c>
+      <c r="L51">
+        <f>J51/1000</f>
+        <v>1.0312354000000001</v>
+      </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" s="2">
         <v>65536</v>
       </c>
@@ -16301,7 +19689,7 @@
         <v>176.019775390625</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" s="5">
         <v>65536</v>
       </c>
@@ -16322,14 +19710,14 @@
         <v>176.0009765625</v>
       </c>
     </row>
-    <row r="56" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C56" s="22"/>
-      <c r="D56" s="22"/>
+    <row r="56" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
     </row>
-    <row r="57" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B57" s="17" t="s">
         <v>6</v>
       </c>
@@ -16349,7 +19737,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" s="2">
         <v>65536</v>
       </c>
@@ -16370,7 +19758,7 @@
         <v>48.076171875</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" s="5">
         <v>65536</v>
       </c>

</xml_diff>

<commit_message>
Fix precision digits in a graph
</commit_message>
<xml_diff>
--- a/measurements/TTT_Graphs.xlsx
+++ b/measurements/TTT_Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\saxion\dotnet\ttt_embedding_languages\measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD6274D-2E96-4FE5-93C5-927E6D26C9D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587B664E-A7D5-4B01-A9B9-3DD6BD57594B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{410AF11E-6A3D-47BB-A088-0867356F1991}"/>
   </bookViews>
@@ -156,7 +156,7 @@
 (allocation of 2 ints, 1 long, 1 DateTime)</t>
   </si>
   <si>
-    <t>in MB / sec</t>
+    <t>in MB and seconds</t>
   </si>
 </sst>
 </file>
@@ -379,6 +379,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,12 +399,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3968,7 +3968,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.23854729115297807"/>
+          <c:y val="0.25623517661818546"/>
+          <c:w val="0.71980107393836024"/>
+          <c:h val="0.58355816277018169"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -4239,6 +4249,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="4.543814717308535E-2"/>
+              <c:y val="0.45624158169696605"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8930,7 +8948,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="#,##0.0\ \µ\s" sourceLinked="0"/>
+            <c:numFmt formatCode="#,##0.00\ \µ\s" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -17914,15 +17932,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>870858</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>903989</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>183460</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>29817</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>16772</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17950,15 +17968,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>861333</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>949520</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4605</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>8844</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>99392</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>22974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18287,7 +18305,7 @@
   <dimension ref="B3:N22"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18302,11 +18320,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -18497,46 +18515,46 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
     </row>
     <row r="17" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="24" t="s">
+      <c r="F17" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24" t="s">
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="25" t="s">
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="26"/>
-      <c r="N17" s="27"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="29"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
       <c r="F18" s="1" t="s">
         <v>9</v>
       </c>
@@ -18775,7 +18793,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:N22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
@@ -18791,11 +18809,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -18986,46 +19004,46 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
     </row>
     <row r="17" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="24" t="s">
+      <c r="F17" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24" t="s">
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="25" t="s">
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="26"/>
-      <c r="N17" s="27"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="29"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
       <c r="F18" s="1" t="s">
         <v>9</v>
       </c>
@@ -19263,8 +19281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC80D5E-FFBA-4A31-8113-D120E3FA18FB}">
   <dimension ref="B34:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="F31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19281,25 +19299,25 @@
   </cols>
   <sheetData>
     <row r="34" spans="2:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="I34" s="28" t="s">
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="I34" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
     </row>
     <row r="35" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="D35" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E35" s="19" t="s">
@@ -19328,9 +19346,9 @@
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
       <c r="E36" s="17" t="s">
         <v>11</v>
       </c>
@@ -19456,11 +19474,11 @@
       </c>
     </row>
     <row r="41" spans="2:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
       <c r="I41" t="s">
         <v>35</v>
       </c>
@@ -19482,13 +19500,13 @@
       </c>
     </row>
     <row r="42" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="24" t="s">
+      <c r="D42" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E42" s="19" t="s">
@@ -19521,9 +19539,9 @@
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
       <c r="E43" s="17" t="s">
         <v>11</v>
       </c>
@@ -19582,7 +19600,7 @@
       <c r="I47" t="s">
         <v>37</v>
       </c>
-      <c r="K47" s="30" t="s">
+      <c r="K47" s="25" t="s">
         <v>38</v>
       </c>
       <c r="L47" t="s">
@@ -19622,11 +19640,11 @@
       </c>
     </row>
     <row r="50" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="28" t="s">
+      <c r="B50" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
       <c r="I50" t="s">
         <v>29</v>
       </c>
@@ -19657,7 +19675,7 @@
       <c r="G51" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I51" s="29" t="s">
+      <c r="I51" s="24" t="s">
         <v>30</v>
       </c>
       <c r="J51">
@@ -19711,11 +19729,11 @@
       </c>
     </row>
     <row r="56" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="28" t="s">
+      <c r="B56" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
     </row>
     <row r="57" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B57" s="17" t="s">

</xml_diff>